<commit_message>
tablas y graficos judicatura fiscalia cites
</commit_message>
<xml_diff>
--- a/55_Entregable tabulados/intermedios/03_cites_tablas.xlsx
+++ b/55_Entregable tabulados/intermedios/03_cites_tablas.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="tabla01" sheetId="1" r:id="rId1"/>
-    <sheet name="tabla02" sheetId="2" r:id="rId2"/>
-    <sheet name="tabla021" sheetId="3" r:id="rId3"/>
-    <sheet name="tabla03" sheetId="4" r:id="rId4"/>
+    <sheet name="registros_permisos_año" sheetId="1" r:id="rId1"/>
+    <sheet name="cantidad_vivos_exportados" sheetId="2" r:id="rId2"/>
+    <sheet name="permisos_vivos_exportados" sheetId="3" r:id="rId3"/>
+    <sheet name="cantidad_sin_vida_exportados" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -457,7 +457,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -471,289 +471,438 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>pais</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>2024</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>2021</t>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="B2">
-        <v>60</v>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Estados Unidos de América</t>
+        </is>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>220</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>11988</v>
+      </c>
+      <c r="F2">
+        <v>83</v>
+      </c>
+      <c r="G2">
+        <v>12396</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CA</t>
-        </is>
-      </c>
-      <c r="B3">
-        <v>11</v>
+          <t>DE</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Alemania</t>
+        </is>
       </c>
       <c r="C3">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>3736</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>4892</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>4892</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CW</t>
-        </is>
-      </c>
-      <c r="B4">
-        <v>0</v>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Canadá</t>
+        </is>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>109</v>
+        <v>63</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>3736</v>
+      </c>
+      <c r="F4">
+        <v>11</v>
+      </c>
+      <c r="G4">
+        <v>3810</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DE</t>
-        </is>
-      </c>
-      <c r="B5">
-        <v>0</v>
+          <t>GB</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Reino Unido</t>
+        </is>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <v>4892</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1168</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1168</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>EC</t>
-        </is>
-      </c>
-      <c r="B6">
-        <v>0</v>
+          <t>SV</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>El Salvador</t>
+        </is>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1083</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1083</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>GB</t>
-        </is>
-      </c>
-      <c r="B7">
-        <v>0</v>
+          <t>TW</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Taiwán, Provincia de China</t>
+        </is>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>1168</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1046</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1046</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>HK</t>
-        </is>
-      </c>
-      <c r="B8">
-        <v>0</v>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Países Bajos</t>
+        </is>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="D8">
-        <v>127</v>
+        <v>40</v>
       </c>
       <c r="E8">
         <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>280</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>KR</t>
-        </is>
-      </c>
-      <c r="B9">
-        <v>0</v>
+          <t>SG</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Singapur</t>
+        </is>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>205</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>205</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>NL</t>
-        </is>
-      </c>
-      <c r="B10">
-        <v>0</v>
+          <t>HK</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Hong Kong (RAE)</t>
+        </is>
       </c>
       <c r="C10">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>240</v>
+        <v>127</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>127</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>PH</t>
-        </is>
-      </c>
-      <c r="B11">
-        <v>0</v>
+          <t>CW</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Curazao</t>
+        </is>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>109</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>109</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>SG</t>
-        </is>
-      </c>
-      <c r="B12">
-        <v>0</v>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>205</v>
+        <v>0</v>
       </c>
       <c r="E12">
         <v>0</v>
+      </c>
+      <c r="F12">
+        <v>60</v>
+      </c>
+      <c r="G12">
+        <v>60</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>SV</t>
-        </is>
-      </c>
-      <c r="B13">
-        <v>0</v>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Filipinas</t>
+        </is>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
-        <v>1083</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>32</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>32</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>TW</t>
-        </is>
-      </c>
-      <c r="B14">
-        <v>0</v>
+          <t>KR</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>República de Corea</t>
+        </is>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>1046</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>27</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>27</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>US</t>
-        </is>
-      </c>
-      <c r="B15">
-        <v>83</v>
+          <t>EC</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Ecuador</t>
+        </is>
       </c>
       <c r="C15">
-        <v>220</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>11988</v>
+        <v>4</v>
       </c>
       <c r="E15">
-        <v>105</v>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C16">
+        <v>345</v>
+      </c>
+      <c r="D16">
+        <v>327</v>
+      </c>
+      <c r="E16">
+        <v>24413</v>
+      </c>
+      <c r="F16">
+        <v>154</v>
+      </c>
+      <c r="G16">
+        <v>25239</v>
       </c>
     </row>
   </sheetData>
@@ -763,7 +912,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -777,42 +926,60 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>pais</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>2024</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>2021</t>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="B2">
-        <v>5</v>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Estados Unidos de América</t>
+        </is>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>34</v>
       </c>
     </row>
     <row r="3">
@@ -821,245 +988,376 @@
           <t>CA</t>
         </is>
       </c>
-      <c r="B3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Canadá</t>
+        </is>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>8</v>
+      </c>
+      <c r="F3">
         <v>1</v>
       </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
+      <c r="G3">
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CW</t>
-        </is>
-      </c>
-      <c r="B4">
-        <v>0</v>
+          <t>DE</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Alemania</t>
+        </is>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DE</t>
-        </is>
-      </c>
-      <c r="B5">
-        <v>0</v>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Países Bajos</t>
+        </is>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E5">
         <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>EC</t>
-        </is>
-      </c>
-      <c r="B6">
-        <v>0</v>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
         <v>0</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>GB</t>
-        </is>
-      </c>
-      <c r="B7">
-        <v>0</v>
+          <t>SG</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Singapur</t>
+        </is>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>HK</t>
-        </is>
-      </c>
-      <c r="B8">
-        <v>0</v>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Filipinas</t>
+        </is>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>KR</t>
-        </is>
-      </c>
-      <c r="B9">
-        <v>0</v>
+          <t>TW</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Taiwán, Provincia de China</t>
+        </is>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>NL</t>
-        </is>
-      </c>
-      <c r="B10">
-        <v>0</v>
+          <t>EC</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Ecuador</t>
+        </is>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>PH</t>
-        </is>
-      </c>
-      <c r="B11">
-        <v>0</v>
+          <t>GB</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Reino Unido</t>
+        </is>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>SG</t>
-        </is>
-      </c>
-      <c r="B12">
-        <v>0</v>
+          <t>CW</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Curazao</t>
+        </is>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>SV</t>
-        </is>
-      </c>
-      <c r="B13">
-        <v>0</v>
+          <t>HK</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Hong Kong (RAE)</t>
+        </is>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
         <v>1</v>
       </c>
-      <c r="E13">
-        <v>0</v>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>TW</t>
-        </is>
-      </c>
-      <c r="B14">
-        <v>0</v>
+          <t>KR</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>República de Corea</t>
+        </is>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>US</t>
-        </is>
-      </c>
-      <c r="B15">
-        <v>2</v>
+          <t>SV</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>El Salvador</t>
+        </is>
       </c>
       <c r="C15">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+      <c r="E16">
+        <v>59</v>
+      </c>
+      <c r="F16">
+        <v>8</v>
+      </c>
+      <c r="G16">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1069,7 +1367,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1083,15 +1381,20 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>cod_unidades</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Elemento</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Muerto</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Sin tipo</t>
         </is>
@@ -1100,80 +1403,105 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Kilogramos (kg)</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>KGM</t>
         </is>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>1131540.85</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
       <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Metros cúbicos (m3)</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>MTQ</t>
         </is>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>65.95</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
       <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
         <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Número de muestras</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>MUE</t>
         </is>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>13330</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>99</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>Número de especímenes</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>NAR</t>
         </is>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>2334</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>580416</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>1094</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>Sin Unidad</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>SIN</t>
         </is>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>17903</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
       <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
         <v>0</v>
       </c>
     </row>

</xml_diff>